<commit_message>
Added DOSUBS, MAP, STREAM
</commit_message>
<xml_diff>
--- a/docs/newRPL Command Database.xlsx
+++ b/docs/newRPL Command Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="827">
   <si>
     <t>!</t>
   </si>
@@ -2496,10 +2496,10 @@
     <t>Percentage completion</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Number of lists param. Is not optional</t>
+  </si>
+  <si>
+    <t>Number of elem. Para. Is not optional</t>
   </si>
 </sst>
 </file>
@@ -2949,8 +2949,8 @@
   <dimension ref="A2:G783"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G214" sqref="G214"/>
+      <pane ySplit="5" topLeftCell="A442" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D768" sqref="D768"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2970,7 +2970,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>COUNTA(D6:D1001)</f>
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>823</v>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="D3" s="8">
         <f>D2/F2</f>
-        <v>9.383033419023136E-2</v>
+        <v>0.10025706940874037</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75">
@@ -6393,11 +6393,9 @@
         <v>787</v>
       </c>
       <c r="E212" s="10"/>
-      <c r="F212" s="10" t="s">
+      <c r="F212" s="10"/>
+      <c r="G212" s="12" t="s">
         <v>825</v>
-      </c>
-      <c r="G212" s="12" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="213" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
@@ -6427,10 +6425,14 @@
       <c r="C214" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D214" s="10"/>
+      <c r="D214" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E214" s="10"/>
       <c r="F214" s="10"/>
-      <c r="G214" s="12"/>
+      <c r="G214" s="12" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="215" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A215" s="10">
@@ -6787,7 +6789,9 @@
       <c r="C236" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D236" s="10"/>
+      <c r="D236" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E236" s="10"/>
       <c r="F236" s="10"/>
       <c r="G236" s="12"/>
@@ -9505,7 +9509,9 @@
       <c r="C404" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D404" s="10"/>
+      <c r="D404" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E404" s="10"/>
       <c r="F404" s="10"/>
       <c r="G404" s="12"/>
@@ -10117,7 +10123,9 @@
       <c r="C442" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D442" s="10"/>
+      <c r="D442" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E442" s="10"/>
       <c r="F442" s="10"/>
       <c r="G442" s="12"/>
@@ -12000,7 +12008,7 @@
       <c r="F559" s="10"/>
       <c r="G559" s="12"/>
     </row>
-    <row r="560" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="560" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A560" s="10">
         <f t="shared" si="8"/>
         <v>555</v>
@@ -12009,7 +12017,7 @@
         <v>502</v>
       </c>
       <c r="C560" s="10" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="D560" s="10"/>
       <c r="E560" s="10"/>
@@ -13589,7 +13597,9 @@
       <c r="C658" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D658" s="10"/>
+      <c r="D658" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E658" s="10"/>
       <c r="F658" s="10"/>
       <c r="G658" s="12"/>
@@ -15699,7 +15709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Added complex number operators.
</commit_message>
<xml_diff>
--- a/docs/newRPL Command Database.xlsx
+++ b/docs/newRPL Command Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1665" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="828">
   <si>
     <t>!</t>
   </si>
@@ -2952,8 +2952,8 @@
   <dimension ref="A2:G783"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A517" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D790" sqref="D790"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2973,7 +2973,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>COUNTA(D6:D1001)</f>
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>823</v>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="D3" s="8">
         <f>D2/F2</f>
-        <v>0.10668380462724936</v>
+        <v>0.11053984575835475</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75">
@@ -3675,7 +3675,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="45" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A45" s="10">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -4067,7 +4067,7 @@
       <c r="F68" s="10"/>
       <c r="G68" s="12"/>
     </row>
-    <row r="69" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="69" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A69" s="10">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -4078,7 +4078,9 @@
       <c r="C69" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D69" s="10"/>
+      <c r="D69" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
       <c r="G69" s="12"/>
@@ -4277,7 +4279,7 @@
       <c r="F81" s="10"/>
       <c r="G81" s="12"/>
     </row>
-    <row r="82" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="82" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A82" s="10">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -4941,7 +4943,7 @@
       <c r="F122" s="10"/>
       <c r="G122" s="12"/>
     </row>
-    <row r="123" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="123" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A123" s="10">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -5459,7 +5461,7 @@
       <c r="F154" s="10"/>
       <c r="G154" s="12"/>
     </row>
-    <row r="155" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="155" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A155" s="10">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -6381,7 +6383,7 @@
       <c r="F211" s="10"/>
       <c r="G211" s="12"/>
     </row>
-    <row r="212" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="212" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A212" s="10">
         <f t="shared" si="3"/>
         <v>207</v>
@@ -6417,7 +6419,7 @@
       <c r="F213" s="10"/>
       <c r="G213" s="12"/>
     </row>
-    <row r="214" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="214" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A214" s="10">
         <f t="shared" si="3"/>
         <v>209</v>
@@ -6781,7 +6783,7 @@
       <c r="F235" s="10"/>
       <c r="G235" s="12"/>
     </row>
-    <row r="236" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="236" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A236" s="10">
         <f t="shared" si="3"/>
         <v>231</v>
@@ -7753,7 +7755,7 @@
       <c r="F295" s="10"/>
       <c r="G295" s="12"/>
     </row>
-    <row r="296" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="296" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A296" s="10">
         <f t="shared" si="4"/>
         <v>291</v>
@@ -7771,7 +7773,7 @@
       <c r="F296" s="10"/>
       <c r="G296" s="12"/>
     </row>
-    <row r="297" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="297" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A297" s="10">
         <f t="shared" si="4"/>
         <v>292</v>
@@ -8013,7 +8015,7 @@
       <c r="F311" s="10"/>
       <c r="G311" s="12"/>
     </row>
-    <row r="312" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="312" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A312" s="10">
         <f t="shared" si="4"/>
         <v>307</v>
@@ -8499,7 +8501,7 @@
       <c r="F341" s="10"/>
       <c r="G341" s="12"/>
     </row>
-    <row r="342" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="342" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A342" s="10">
         <f t="shared" si="5"/>
         <v>337</v>
@@ -9241,7 +9243,7 @@
       <c r="F387" s="10"/>
       <c r="G387" s="12"/>
     </row>
-    <row r="388" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="388" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A388" s="10">
         <f t="shared" si="5"/>
         <v>383</v>
@@ -9501,7 +9503,7 @@
       <c r="F403" s="10"/>
       <c r="G403" s="12"/>
     </row>
-    <row r="404" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="404" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A404" s="10">
         <f t="shared" si="6"/>
         <v>399</v>
@@ -10117,7 +10119,7 @@
       <c r="F441" s="10"/>
       <c r="G441" s="12"/>
     </row>
-    <row r="442" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="442" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A442" s="10">
         <f t="shared" si="6"/>
         <v>437</v>
@@ -11321,7 +11323,7 @@
       <c r="F516" s="10"/>
       <c r="G516" s="12"/>
     </row>
-    <row r="517" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="517" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A517" s="10">
         <f t="shared" si="7"/>
         <v>512</v>
@@ -11339,7 +11341,7 @@
       <c r="F517" s="10"/>
       <c r="G517" s="12"/>
     </row>
-    <row r="518" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="518" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A518" s="10">
         <f t="shared" si="7"/>
         <v>513</v>
@@ -11533,7 +11535,7 @@
       <c r="F529" s="10"/>
       <c r="G529" s="12"/>
     </row>
-    <row r="530" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="530" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A530" s="10">
         <f t="shared" si="8"/>
         <v>525</v>
@@ -11869,7 +11871,7 @@
       <c r="F550" s="10"/>
       <c r="G550" s="12"/>
     </row>
-    <row r="551" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="551" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A551" s="10">
         <f t="shared" si="8"/>
         <v>546</v>
@@ -12079,7 +12081,7 @@
       <c r="F563" s="10"/>
       <c r="G563" s="12"/>
     </row>
-    <row r="564" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="564" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A564" s="10">
         <f t="shared" si="8"/>
         <v>559</v>
@@ -12090,7 +12092,9 @@
       <c r="C564" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D564" s="10"/>
+      <c r="D564" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E564" s="10"/>
       <c r="F564" s="10"/>
       <c r="G564" s="12"/>
@@ -12751,7 +12755,7 @@
       <c r="F605" s="10"/>
       <c r="G605" s="12"/>
     </row>
-    <row r="606" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="606" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A606" s="10">
         <f t="shared" si="9"/>
         <v>601</v>
@@ -13187,7 +13191,7 @@
       <c r="F632" s="10"/>
       <c r="G632" s="12"/>
     </row>
-    <row r="633" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="633" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A633" s="10">
         <f t="shared" si="9"/>
         <v>628</v>
@@ -13198,7 +13202,9 @@
       <c r="C633" s="10" t="s">
         <v>795</v>
       </c>
-      <c r="D633" s="10"/>
+      <c r="D633" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E633" s="10"/>
       <c r="F633" s="10"/>
       <c r="G633" s="12"/>
@@ -13593,7 +13599,7 @@
       <c r="F657" s="10"/>
       <c r="G657" s="12"/>
     </row>
-    <row r="658" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="658" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A658" s="10">
         <f t="shared" si="10"/>
         <v>653</v>
@@ -13837,7 +13843,7 @@
       <c r="F672" s="10"/>
       <c r="G672" s="12"/>
     </row>
-    <row r="673" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="673" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A673" s="10">
         <f t="shared" si="10"/>
         <v>668</v>
@@ -15053,7 +15059,7 @@
       <c r="F747" s="10"/>
       <c r="G747" s="12"/>
     </row>
-    <row r="748" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="748" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A748" s="10">
         <f t="shared" si="11"/>
         <v>743</v>
@@ -15373,7 +15379,7 @@
       <c r="F767" s="10"/>
       <c r="G767" s="12"/>
     </row>
-    <row r="768" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="768" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A768" s="10">
         <f t="shared" si="11"/>
         <v>763</v>
@@ -15407,7 +15413,7 @@
       <c r="F769" s="10"/>
       <c r="G769" s="12"/>
     </row>
-    <row r="770" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="770" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A770" s="10">
         <f t="shared" si="11"/>
         <v>765</v>
@@ -15491,7 +15497,7 @@
       <c r="F774" s="10"/>
       <c r="G774" s="12"/>
     </row>
-    <row r="775" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="775" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A775" s="10">
         <f t="shared" ref="A775:A783" si="12">A774+1</f>
         <v>770</v>
@@ -15643,7 +15649,7 @@
   <autoFilter ref="A5:G783">
     <filterColumn colId="2">
       <filters>
-        <filter val="Lists"/>
+        <filter val="Complex"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Added basic support for symbolics to the compiler.
</commit_message>
<xml_diff>
--- a/docs/newRPL Command Database.xlsx
+++ b/docs/newRPL Command Database.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="828">
   <si>
     <t>!</t>
   </si>
@@ -2953,7 +2953,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+      <selection pane="bottomLeft" activeCell="D223" sqref="D223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2973,7 +2973,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="7">
         <f>COUNTA(D6:D1001)</f>
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>823</v>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="D3" s="8">
         <f>D2/F2</f>
-        <v>0.11053984575835475</v>
+        <v>0.12339331619537275</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75">
@@ -3800,12 +3800,14 @@
       <c r="C52" s="10" t="s">
         <v>791</v>
       </c>
-      <c r="D52" s="10"/>
+      <c r="D52" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="12"/>
     </row>
-    <row r="53" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="53" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A53" s="10">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4279,7 +4281,7 @@
       <c r="F81" s="10"/>
       <c r="G81" s="12"/>
     </row>
-    <row r="82" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="82" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A82" s="10">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -4290,7 +4292,9 @@
       <c r="C82" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="D82" s="10"/>
+      <c r="D82" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E82" s="10"/>
       <c r="F82" s="10"/>
       <c r="G82" s="12"/>
@@ -4943,7 +4947,7 @@
       <c r="F122" s="10"/>
       <c r="G122" s="12"/>
     </row>
-    <row r="123" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="123" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A123" s="10">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -4954,7 +4958,9 @@
       <c r="C123" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="D123" s="10"/>
+      <c r="D123" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E123" s="10"/>
       <c r="F123" s="10"/>
       <c r="G123" s="12"/>
@@ -5461,7 +5467,7 @@
       <c r="F154" s="10"/>
       <c r="G154" s="12"/>
     </row>
-    <row r="155" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="155" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A155" s="10">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -5472,7 +5478,9 @@
       <c r="C155" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="D155" s="10"/>
+      <c r="D155" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E155" s="10"/>
       <c r="F155" s="10"/>
       <c r="G155" s="12"/>
@@ -6569,7 +6577,7 @@
       <c r="F222" s="10"/>
       <c r="G222" s="12"/>
     </row>
-    <row r="223" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
+    <row r="223" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
       <c r="A223" s="10">
         <f t="shared" si="3"/>
         <v>218</v>
@@ -8220,7 +8228,9 @@
       <c r="C324" s="10" t="s">
         <v>805</v>
       </c>
-      <c r="D324" s="10"/>
+      <c r="D324" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E324" s="10"/>
       <c r="F324" s="10"/>
       <c r="G324" s="12"/>
@@ -8501,7 +8511,7 @@
       <c r="F341" s="10"/>
       <c r="G341" s="12"/>
     </row>
-    <row r="342" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="342" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A342" s="10">
         <f t="shared" si="5"/>
         <v>337</v>
@@ -8512,7 +8522,9 @@
       <c r="C342" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="D342" s="10"/>
+      <c r="D342" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E342" s="10"/>
       <c r="F342" s="10"/>
       <c r="G342" s="12"/>
@@ -11535,7 +11547,7 @@
       <c r="F529" s="10"/>
       <c r="G529" s="12"/>
     </row>
-    <row r="530" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="530" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A530" s="10">
         <f t="shared" si="8"/>
         <v>525</v>
@@ -11546,7 +11558,9 @@
       <c r="C530" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="D530" s="10"/>
+      <c r="D530" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E530" s="10"/>
       <c r="F530" s="10"/>
       <c r="G530" s="12"/>
@@ -11871,7 +11885,7 @@
       <c r="F550" s="10"/>
       <c r="G550" s="12"/>
     </row>
-    <row r="551" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="551" spans="1:7" s="9" customFormat="1" ht="24" hidden="1" customHeight="1">
       <c r="A551" s="10">
         <f t="shared" si="8"/>
         <v>546</v>
@@ -11882,7 +11896,9 @@
       <c r="C551" s="10" t="s">
         <v>801</v>
       </c>
-      <c r="D551" s="10"/>
+      <c r="D551" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E551" s="10"/>
       <c r="F551" s="10"/>
       <c r="G551" s="12"/>
@@ -12542,7 +12558,9 @@
       <c r="C592" s="10" t="s">
         <v>789</v>
       </c>
-      <c r="D592" s="10"/>
+      <c r="D592" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E592" s="10"/>
       <c r="F592" s="10"/>
       <c r="G592" s="12"/>
@@ -15086,7 +15104,9 @@
       <c r="C749" s="10" t="s">
         <v>797</v>
       </c>
-      <c r="D749" s="10"/>
+      <c r="D749" s="10" t="s">
+        <v>787</v>
+      </c>
       <c r="E749" s="10"/>
       <c r="F749" s="10"/>
       <c r="G749" s="12"/>
@@ -15649,7 +15669,7 @@
   <autoFilter ref="A5:G783">
     <filterColumn colId="2">
       <filters>
-        <filter val="Complex"/>
+        <filter val="Tags"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>